<commit_message>
arbejde på show all Members
</commit_message>
<xml_diff>
--- a/Delfinen Svømmeklub Medlemsliste.xlsx
+++ b/Delfinen Svømmeklub Medlemsliste.xlsx
@@ -1,13 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Delfinen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA8988D-EEE7-4B77-88FF-B1D83C7F6BEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -470,88 +490,388 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.57"/>
-    <col customWidth="1" min="2" max="2" width="8.86"/>
-    <col customWidth="1" min="3" max="3" width="11.0"/>
-    <col customWidth="1" min="4" max="4" width="21.0"/>
-    <col customWidth="1" min="5" max="5" width="7.0"/>
-    <col customWidth="1" min="6" max="6" width="12.43"/>
-    <col customWidth="1" min="7" max="7" width="4.71"/>
-    <col customWidth="1" min="8" max="8" width="12.14"/>
-    <col customWidth="1" min="9" max="9" width="12.86"/>
-    <col customWidth="1" min="10" max="10" width="7.14"/>
-    <col customWidth="1" min="11" max="11" width="11.43"/>
-    <col customWidth="1" min="12" max="12" width="8.43"/>
-    <col customWidth="1" min="13" max="13" width="4.43"/>
-    <col customWidth="1" min="14" max="14" width="8.43"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="4.42578125" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,9 +915,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -609,7 +929,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -624,15 +944,15 @@
         <v>20</v>
       </c>
       <c r="J3" s="2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="K3" s="3">
-        <v>100200.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>100200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
@@ -644,7 +964,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>17</v>
@@ -659,7 +979,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="2">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>26</v>
@@ -668,12 +988,12 @@
         <v>26</v>
       </c>
       <c r="M4" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
@@ -685,7 +1005,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
@@ -700,21 +1020,21 @@
         <v>25</v>
       </c>
       <c r="J5" s="2">
-        <v>2002.0</v>
+        <v>2002</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L5" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N5" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>31</v>
@@ -726,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="E6" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>17</v>
@@ -741,21 +1061,21 @@
         <v>25</v>
       </c>
       <c r="J6" s="2">
-        <v>2005.0</v>
+        <v>2005</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L6" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M6" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
@@ -767,7 +1087,7 @@
         <v>36</v>
       </c>
       <c r="E7" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
@@ -782,21 +1102,21 @@
         <v>25</v>
       </c>
       <c r="J7" s="2">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L7" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N7" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>37</v>
@@ -808,7 +1128,7 @@
         <v>38</v>
       </c>
       <c r="E8" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
@@ -823,21 +1143,21 @@
         <v>25</v>
       </c>
       <c r="J8" s="2">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N8" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>40</v>
@@ -849,7 +1169,7 @@
         <v>42</v>
       </c>
       <c r="E9" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>17</v>
@@ -864,12 +1184,12 @@
         <v>20</v>
       </c>
       <c r="J9" s="2">
-        <v>1998.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>43</v>
@@ -881,7 +1201,7 @@
         <v>45</v>
       </c>
       <c r="E10" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
@@ -896,21 +1216,21 @@
         <v>25</v>
       </c>
       <c r="J10" s="2">
-        <v>1995.0</v>
+        <v>1995</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L10" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M10" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>46</v>
@@ -922,7 +1242,7 @@
         <v>48</v>
       </c>
       <c r="E11" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
@@ -937,7 +1257,7 @@
         <v>25</v>
       </c>
       <c r="J11" s="2">
-        <v>1996.0</v>
+        <v>1996</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>26</v>
@@ -946,12 +1266,12 @@
         <v>26</v>
       </c>
       <c r="M11" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>49</v>
@@ -963,7 +1283,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
@@ -978,7 +1298,7 @@
         <v>25</v>
       </c>
       <c r="J12" s="2">
-        <v>1996.0</v>
+        <v>1996</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>26</v>
@@ -987,12 +1307,12 @@
         <v>26</v>
       </c>
       <c r="M12" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>51</v>
@@ -1004,7 +1324,7 @@
         <v>52</v>
       </c>
       <c r="E13" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
@@ -1019,21 +1339,21 @@
         <v>25</v>
       </c>
       <c r="J13" s="2">
-        <v>1970.0</v>
+        <v>1970</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L13" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M13" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>53</v>
@@ -1045,7 +1365,7 @@
         <v>55</v>
       </c>
       <c r="E14" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>17</v>
@@ -1060,21 +1380,21 @@
         <v>25</v>
       </c>
       <c r="J14" s="2">
-        <v>1975.0</v>
+        <v>1975</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N14" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>56</v>
@@ -1086,7 +1406,7 @@
         <v>57</v>
       </c>
       <c r="E15" s="2">
-        <v>3760.0</v>
+        <v>3760</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>58</v>
@@ -1101,7 +1421,7 @@
         <v>25</v>
       </c>
       <c r="J15" s="2">
-        <v>1980.0</v>
+        <v>1980</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>59</v>
@@ -1110,15 +1430,15 @@
         <v>26</v>
       </c>
       <c r="M15" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>60</v>
@@ -1130,7 +1450,7 @@
         <v>62</v>
       </c>
       <c r="E16" s="2">
-        <v>3730.0</v>
+        <v>3730</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>63</v>
@@ -1145,21 +1465,21 @@
         <v>25</v>
       </c>
       <c r="J16" s="2">
-        <v>1985.0</v>
+        <v>1985</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L16" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N16" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>64</v>
@@ -1171,7 +1491,7 @@
         <v>65</v>
       </c>
       <c r="E17" s="2">
-        <v>3740.0</v>
+        <v>3740</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>66</v>
@@ -1186,21 +1506,21 @@
         <v>25</v>
       </c>
       <c r="J17" s="2">
-        <v>1990.0</v>
+        <v>1990</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L17" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M17" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
@@ -1212,7 +1532,7 @@
         <v>68</v>
       </c>
       <c r="E18" s="2">
-        <v>3740.0</v>
+        <v>3740</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>66</v>
@@ -1227,12 +1547,12 @@
         <v>20</v>
       </c>
       <c r="J18" s="2">
-        <v>1950.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>69</v>
@@ -1244,7 +1564,7 @@
         <v>71</v>
       </c>
       <c r="E19" s="2">
-        <v>3730.0</v>
+        <v>3730</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>63</v>
@@ -1259,7 +1579,7 @@
         <v>25</v>
       </c>
       <c r="J19" s="2">
-        <v>1955.0</v>
+        <v>1955</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>59</v>
@@ -1268,15 +1588,15 @@
         <v>26</v>
       </c>
       <c r="M19" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>72</v>
@@ -1288,7 +1608,7 @@
         <v>74</v>
       </c>
       <c r="E20" s="2">
-        <v>3760.0</v>
+        <v>3760</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>58</v>
@@ -1303,21 +1623,21 @@
         <v>25</v>
       </c>
       <c r="J20" s="2">
-        <v>1958.0</v>
+        <v>1958</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L20" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M20" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>75</v>
@@ -1329,7 +1649,7 @@
         <v>76</v>
       </c>
       <c r="E21" s="2">
-        <v>3740.0</v>
+        <v>3740</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>66</v>
@@ -1344,7 +1664,7 @@
         <v>25</v>
       </c>
       <c r="J21" s="2">
-        <v>1959.0</v>
+        <v>1959</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>59</v>
@@ -1353,15 +1673,15 @@
         <v>26</v>
       </c>
       <c r="M21" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>46</v>
@@ -1373,7 +1693,7 @@
         <v>78</v>
       </c>
       <c r="E22" s="2">
-        <v>3770.0</v>
+        <v>3770</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>79</v>
@@ -1388,7 +1708,7 @@
         <v>25</v>
       </c>
       <c r="J22" s="2">
-        <v>1960.0</v>
+        <v>1960</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>26</v>
@@ -1397,12 +1717,12 @@
         <v>26</v>
       </c>
       <c r="M22" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>80</v>
@@ -1414,7 +1734,7 @@
         <v>81</v>
       </c>
       <c r="E23" s="2">
-        <v>3740.0</v>
+        <v>3740</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>66</v>
@@ -1429,21 +1749,21 @@
         <v>25</v>
       </c>
       <c r="J23" s="2">
-        <v>1954.0</v>
+        <v>1954</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L23" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M23" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>82</v>
@@ -1455,7 +1775,7 @@
         <v>83</v>
       </c>
       <c r="E24" s="2">
-        <v>3760.0</v>
+        <v>3760</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>58</v>
@@ -1470,7 +1790,7 @@
         <v>25</v>
       </c>
       <c r="J24" s="2">
-        <v>1943.0</v>
+        <v>1943</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>59</v>
@@ -1479,15 +1799,15 @@
         <v>26</v>
       </c>
       <c r="M24" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>84</v>
@@ -1499,7 +1819,7 @@
         <v>86</v>
       </c>
       <c r="E25" s="2">
-        <v>3782.0</v>
+        <v>3782</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>87</v>
@@ -1514,21 +1834,21 @@
         <v>25</v>
       </c>
       <c r="J25" s="2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L25" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N25" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>88</v>
@@ -1540,7 +1860,7 @@
         <v>89</v>
       </c>
       <c r="E26" s="2">
-        <v>3730.0</v>
+        <v>3730</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>63</v>
@@ -1555,7 +1875,7 @@
         <v>25</v>
       </c>
       <c r="J26" s="2">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>26</v>
@@ -1564,12 +1884,12 @@
         <v>26</v>
       </c>
       <c r="M26" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>90</v>
@@ -1581,7 +1901,7 @@
         <v>91</v>
       </c>
       <c r="E27" s="2">
-        <v>3782.0</v>
+        <v>3782</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>87</v>
@@ -1596,12 +1916,12 @@
         <v>20</v>
       </c>
       <c r="J27" s="2">
-        <v>2002.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>92</v>
@@ -1613,7 +1933,7 @@
         <v>93</v>
       </c>
       <c r="E28" s="2">
-        <v>3760.0</v>
+        <v>3760</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>58</v>
@@ -1628,7 +1948,7 @@
         <v>25</v>
       </c>
       <c r="J28" s="2">
-        <v>2005.0</v>
+        <v>2005</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>59</v>
@@ -1637,15 +1957,15 @@
         <v>26</v>
       </c>
       <c r="M28" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>94</v>
@@ -1657,7 +1977,7 @@
         <v>96</v>
       </c>
       <c r="E29" s="2">
-        <v>3782.0</v>
+        <v>3782</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>87</v>
@@ -1672,21 +1992,21 @@
         <v>25</v>
       </c>
       <c r="J29" s="2">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L29" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N29" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>97</v>
@@ -1698,7 +2018,7 @@
         <v>98</v>
       </c>
       <c r="E30" s="2">
-        <v>3782.0</v>
+        <v>3782</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>87</v>
@@ -1713,7 +2033,7 @@
         <v>25</v>
       </c>
       <c r="J30" s="2">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>26</v>
@@ -1722,12 +2042,12 @@
         <v>26</v>
       </c>
       <c r="M30" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>99</v>
@@ -1739,7 +2059,7 @@
         <v>100</v>
       </c>
       <c r="E31" s="2">
-        <v>3782.0</v>
+        <v>3782</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>87</v>
@@ -1754,21 +2074,21 @@
         <v>25</v>
       </c>
       <c r="J31" s="2">
-        <v>1980.0</v>
+        <v>1980</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L31" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M31" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>101</v>
@@ -1780,7 +2100,7 @@
         <v>102</v>
       </c>
       <c r="E32" s="2">
-        <v>3760.0</v>
+        <v>3760</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>58</v>
@@ -1795,7 +2115,7 @@
         <v>25</v>
       </c>
       <c r="J32" s="2">
-        <v>1985.0</v>
+        <v>1985</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>59</v>
@@ -1804,15 +2124,15 @@
         <v>26</v>
       </c>
       <c r="M32" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>103</v>
@@ -1824,7 +2144,7 @@
         <v>105</v>
       </c>
       <c r="E33" s="2">
-        <v>3770.0</v>
+        <v>3770</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>79</v>
@@ -1839,21 +2159,21 @@
         <v>25</v>
       </c>
       <c r="J33" s="2">
-        <v>1990.0</v>
+        <v>1990</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L33" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N33" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>106</v>
@@ -1865,7 +2185,7 @@
         <v>107</v>
       </c>
       <c r="E34" s="2">
-        <v>3740.0</v>
+        <v>3740</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>66</v>
@@ -1880,7 +2200,7 @@
         <v>25</v>
       </c>
       <c r="J34" s="2">
-        <v>1950.0</v>
+        <v>1950</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>59</v>
@@ -1889,15 +2209,15 @@
         <v>26</v>
       </c>
       <c r="M34" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>108</v>
@@ -1909,7 +2229,7 @@
         <v>109</v>
       </c>
       <c r="E35" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>17</v>
@@ -1924,21 +2244,21 @@
         <v>25</v>
       </c>
       <c r="J35" s="2">
-        <v>1955.0</v>
+        <v>1955</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L35" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M35" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>110</v>
@@ -1950,7 +2270,7 @@
         <v>111</v>
       </c>
       <c r="E36" s="2">
-        <v>3770.0</v>
+        <v>3770</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>79</v>
@@ -1965,12 +2285,12 @@
         <v>20</v>
       </c>
       <c r="J36" s="2">
-        <v>1958.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>112</v>
@@ -1982,7 +2302,7 @@
         <v>114</v>
       </c>
       <c r="E37" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>17</v>
@@ -1997,7 +2317,7 @@
         <v>25</v>
       </c>
       <c r="J37" s="2">
-        <v>1959.0</v>
+        <v>1959</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>59</v>
@@ -2006,15 +2326,15 @@
         <v>26</v>
       </c>
       <c r="M37" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>115</v>
@@ -2026,7 +2346,7 @@
         <v>116</v>
       </c>
       <c r="E38" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>17</v>
@@ -2041,7 +2361,7 @@
         <v>25</v>
       </c>
       <c r="J38" s="2">
-        <v>1980.0</v>
+        <v>1980</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>26</v>
@@ -2050,12 +2370,12 @@
         <v>26</v>
       </c>
       <c r="M38" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>117</v>
@@ -2067,7 +2387,7 @@
         <v>119</v>
       </c>
       <c r="E39" s="2">
-        <v>3760.0</v>
+        <v>3760</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>58</v>
@@ -2082,7 +2402,7 @@
         <v>25</v>
       </c>
       <c r="J39" s="2">
-        <v>1985.0</v>
+        <v>1985</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>59</v>
@@ -2091,15 +2411,15 @@
         <v>26</v>
       </c>
       <c r="M39" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>120</v>
@@ -2111,7 +2431,7 @@
         <v>121</v>
       </c>
       <c r="E40" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>17</v>
@@ -2126,21 +2446,21 @@
         <v>25</v>
       </c>
       <c r="J40" s="2">
-        <v>1990.0</v>
+        <v>1990</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L40" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N40" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>122</v>
@@ -2152,7 +2472,7 @@
         <v>124</v>
       </c>
       <c r="E41" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>17</v>
@@ -2167,7 +2487,7 @@
         <v>25</v>
       </c>
       <c r="J41" s="2">
-        <v>1950.0</v>
+        <v>1950</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>59</v>
@@ -2176,15 +2496,15 @@
         <v>26</v>
       </c>
       <c r="M41" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N41" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>125</v>
@@ -2196,7 +2516,7 @@
         <v>126</v>
       </c>
       <c r="E42" s="2">
-        <v>3730.0</v>
+        <v>3730</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>63</v>
@@ -2211,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="J42" s="2">
-        <v>1955.0</v>
+        <v>1955</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>59</v>
@@ -2220,15 +2540,15 @@
         <v>26</v>
       </c>
       <c r="M42" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N42" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>127</v>
@@ -2240,7 +2560,7 @@
         <v>129</v>
       </c>
       <c r="E43" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>17</v>
@@ -2255,21 +2575,21 @@
         <v>25</v>
       </c>
       <c r="J43" s="2">
-        <v>1958.0</v>
+        <v>1958</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L43" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N43" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>130</v>
@@ -2281,7 +2601,7 @@
         <v>131</v>
       </c>
       <c r="E44" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>17</v>
@@ -2296,7 +2616,7 @@
         <v>25</v>
       </c>
       <c r="J44" s="2">
-        <v>1959.0</v>
+        <v>1959</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>26</v>
@@ -2305,12 +2625,12 @@
         <v>26</v>
       </c>
       <c r="M44" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>132</v>
@@ -2322,7 +2642,7 @@
         <v>134</v>
       </c>
       <c r="E45" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>17</v>
@@ -2337,12 +2657,12 @@
         <v>20</v>
       </c>
       <c r="J45" s="2">
-        <v>2002.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>135</v>
@@ -2354,7 +2674,7 @@
         <v>136</v>
       </c>
       <c r="E46" s="2">
-        <v>3700.0</v>
+        <v>3700</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>17</v>
@@ -2369,7 +2689,7 @@
         <v>25</v>
       </c>
       <c r="J46" s="2">
-        <v>2005.0</v>
+        <v>2005</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>26</v>
@@ -2378,12 +2698,12 @@
         <v>26</v>
       </c>
       <c r="M46" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>137</v>
@@ -2395,7 +2715,7 @@
         <v>139</v>
       </c>
       <c r="E47" s="2">
-        <v>3770.0</v>
+        <v>3770</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>79</v>
@@ -2410,7 +2730,7 @@
         <v>25</v>
       </c>
       <c r="J47" s="2">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>26</v>
@@ -2419,12 +2739,12 @@
         <v>26</v>
       </c>
       <c r="M47" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>140</v>
@@ -2436,7 +2756,7 @@
         <v>142</v>
       </c>
       <c r="E48" s="2">
-        <v>3770.0</v>
+        <v>3770</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>79</v>
@@ -2451,21 +2771,21 @@
         <v>25</v>
       </c>
       <c r="J48" s="2">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L48" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="M48" s="2">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>143</v>
@@ -2477,7 +2797,7 @@
         <v>145</v>
       </c>
       <c r="E49" s="2">
-        <v>3730.0</v>
+        <v>3730</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>63</v>
@@ -2492,7 +2812,7 @@
         <v>25</v>
       </c>
       <c r="J49" s="2">
-        <v>1998.0</v>
+        <v>1998</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>59</v>
@@ -2501,15 +2821,15 @@
         <v>26</v>
       </c>
       <c r="M49" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>146</v>
@@ -2521,7 +2841,7 @@
         <v>147</v>
       </c>
       <c r="E50" s="2">
-        <v>3770.0</v>
+        <v>3770</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>79</v>
@@ -2536,7 +2856,7 @@
         <v>25</v>
       </c>
       <c r="J50" s="2">
-        <v>1995.0</v>
+        <v>1995</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>26</v>
@@ -2545,12 +2865,12 @@
         <v>26</v>
       </c>
       <c r="M50" s="2">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>148</v>
@@ -2562,7 +2882,7 @@
         <v>150</v>
       </c>
       <c r="E51" s="2">
-        <v>3770.0</v>
+        <v>3770</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>79</v>
@@ -2577,25 +2897,26 @@
         <v>20</v>
       </c>
       <c r="J51" s="2">
-        <v>2004.0</v>
+        <v>2004</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <f>Sheet1!A3</f>
         <v>1</v>
@@ -2617,15 +2938,15 @@
         <v>2000</v>
       </c>
       <c r="F1">
-        <f>if(Sheet1!I3 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I3 = "motionist",2,1)</f>
         <v>2</v>
       </c>
       <c r="G1">
-        <f>if(Sheet1!H3 = "passiv",0,1)</f>
+        <f>IF(Sheet1!H3 = "passiv",0,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>Sheet1!A4</f>
         <v>2</v>
@@ -2647,15 +2968,15 @@
         <v>2001</v>
       </c>
       <c r="F2">
-        <f>if(Sheet1!I4 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I4 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G2">
-        <f>if(Sheet1!H4 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
+        <f>IF(Sheet1!H4 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>Sheet1!A5</f>
         <v>3</v>
@@ -2677,15 +2998,15 @@
         <v>2002</v>
       </c>
       <c r="F3">
-        <f>if(Sheet1!I5 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I5 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G3">
-        <f>if(Sheet1!H5 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
+        <f>IF(Sheet1!H5 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>Sheet1!A6</f>
         <v>4</v>
@@ -2707,15 +3028,15 @@
         <v>2005</v>
       </c>
       <c r="F4">
-        <f>if(Sheet1!I6 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I6 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G4">
-        <f>if(Sheet1!H6 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
+        <f>IF(Sheet1!H6 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>Sheet1!A7</f>
         <v>5</v>
@@ -2737,15 +3058,15 @@
         <v>1999</v>
       </c>
       <c r="F5">
-        <f>if(Sheet1!I7 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I7 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G5">
-        <f>if(Sheet1!H7 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
+        <f>IF(Sheet1!H7 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>Sheet1!A8</f>
         <v>6</v>
@@ -2767,15 +3088,15 @@
         <v>1999</v>
       </c>
       <c r="F6">
-        <f>if(Sheet1!I8 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I8 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G6">
-        <f>if(Sheet1!H8 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
+        <f>IF(Sheet1!H8 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>Sheet1!A9</f>
         <v>7</v>
@@ -2797,15 +3118,15 @@
         <v>1998</v>
       </c>
       <c r="F7">
-        <f>if(Sheet1!I9 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I9 = "motionist",2,1)</f>
         <v>2</v>
       </c>
       <c r="G7">
-        <f>if(Sheet1!H9 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
+        <f>IF(Sheet1!H9 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>Sheet1!A10</f>
         <v>8</v>
@@ -2827,15 +3148,15 @@
         <v>1995</v>
       </c>
       <c r="F8">
-        <f>if(Sheet1!I10 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I10 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G8">
-        <f>if(Sheet1!H10 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
+        <f>IF(Sheet1!H10 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <f>Sheet1!A11</f>
         <v>9</v>
@@ -2857,15 +3178,15 @@
         <v>1996</v>
       </c>
       <c r="F9">
-        <f>if(Sheet1!I11 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I11 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G9">
-        <f>if(Sheet1!H11 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
+        <f>IF(Sheet1!H11 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>Sheet1!A12</f>
         <v>10</v>
@@ -2887,15 +3208,15 @@
         <v>1996</v>
       </c>
       <c r="F10">
-        <f>if(Sheet1!I12 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I12 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G10">
-        <f>if(Sheet1!H12 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
+        <f>IF(Sheet1!H12 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f>Sheet1!A13</f>
         <v>11</v>
@@ -2917,15 +3238,15 @@
         <v>1970</v>
       </c>
       <c r="F11">
-        <f>if(Sheet1!I13 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I13 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G11">
-        <f>if(Sheet1!H13 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
+        <f>IF(Sheet1!H13 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f>Sheet1!A14</f>
         <v>12</v>
@@ -2947,15 +3268,15 @@
         <v>1975</v>
       </c>
       <c r="F12">
-        <f>if(Sheet1!I14 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I14 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G12">
-        <f>if(Sheet1!H14 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
+        <f>IF(Sheet1!H14 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>Sheet1!A15</f>
         <v>13</v>
@@ -2977,15 +3298,15 @@
         <v>1980</v>
       </c>
       <c r="F13">
-        <f>if(Sheet1!I15 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I15 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G13">
-        <f>if(Sheet1!H15 = "passiv",0,1)</f>
+        <f>IF(Sheet1!H15 = "passiv",0,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <f>Sheet1!A16</f>
         <v>14</v>
@@ -3007,15 +3328,15 @@
         <v>1985</v>
       </c>
       <c r="F14">
-        <f>if(Sheet1!I16 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I16 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G14">
-        <f>if(Sheet1!H16 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
+        <f>IF(Sheet1!H16 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>Sheet1!A17</f>
         <v>15</v>
@@ -3037,15 +3358,15 @@
         <v>1990</v>
       </c>
       <c r="F15">
-        <f>if(Sheet1!I17 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I17 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G15">
-        <f>if(Sheet1!H17 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
+        <f>IF(Sheet1!H17 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <f>Sheet1!A18</f>
         <v>16</v>
@@ -3067,15 +3388,15 @@
         <v>1950</v>
       </c>
       <c r="F16">
-        <f>if(Sheet1!I18 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I18 = "motionist",2,1)</f>
         <v>2</v>
       </c>
       <c r="G16">
-        <f>if(Sheet1!H18 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
+        <f>IF(Sheet1!H18 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>Sheet1!A19</f>
         <v>17</v>
@@ -3097,15 +3418,15 @@
         <v>1955</v>
       </c>
       <c r="F17">
-        <f>if(Sheet1!I19 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I19 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G17">
-        <f>if(Sheet1!H19 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
+        <f>IF(Sheet1!H19 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>Sheet1!A20</f>
         <v>18</v>
@@ -3127,15 +3448,15 @@
         <v>1958</v>
       </c>
       <c r="F18">
-        <f>if(Sheet1!I20 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I20 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G18">
-        <f>if(Sheet1!H20 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
+        <f>IF(Sheet1!H20 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>Sheet1!A21</f>
         <v>19</v>
@@ -3157,15 +3478,15 @@
         <v>1959</v>
       </c>
       <c r="F19">
-        <f>if(Sheet1!I21 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I21 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G19">
-        <f>if(Sheet1!H21 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
+        <f>IF(Sheet1!H21 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>Sheet1!A22</f>
         <v>20</v>
@@ -3187,15 +3508,15 @@
         <v>1960</v>
       </c>
       <c r="F20">
-        <f>if(Sheet1!I22 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I22 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G20">
-        <f>if(Sheet1!H22 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
+        <f>IF(Sheet1!H22 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>Sheet1!A23</f>
         <v>21</v>
@@ -3217,15 +3538,15 @@
         <v>1954</v>
       </c>
       <c r="F21">
-        <f>if(Sheet1!I23 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I23 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G21">
-        <f>if(Sheet1!H23 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
+        <f>IF(Sheet1!H23 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>Sheet1!A24</f>
         <v>22</v>
@@ -3247,15 +3568,15 @@
         <v>1943</v>
       </c>
       <c r="F22">
-        <f>if(Sheet1!I24 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I24 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G22">
-        <f>if(Sheet1!H24 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
+        <f>IF(Sheet1!H24 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>Sheet1!A25</f>
         <v>23</v>
@@ -3277,15 +3598,15 @@
         <v>2000</v>
       </c>
       <c r="F23">
-        <f>if(Sheet1!I25 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I25 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G23">
-        <f>if(Sheet1!H25 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
+        <f>IF(Sheet1!H25 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>Sheet1!A26</f>
         <v>24</v>
@@ -3307,15 +3628,15 @@
         <v>2001</v>
       </c>
       <c r="F24">
-        <f>if(Sheet1!I26 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I26 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G24">
-        <f>if(Sheet1!H26 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
+        <f>IF(Sheet1!H26 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>Sheet1!A27</f>
         <v>25</v>
@@ -3337,15 +3658,15 @@
         <v>2002</v>
       </c>
       <c r="F25">
-        <f>if(Sheet1!I27 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I27 = "motionist",2,1)</f>
         <v>2</v>
       </c>
       <c r="G25">
-        <f>if(Sheet1!H27 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
+        <f>IF(Sheet1!H27 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>Sheet1!A28</f>
         <v>26</v>
@@ -3367,15 +3688,15 @@
         <v>2005</v>
       </c>
       <c r="F26">
-        <f>if(Sheet1!I28 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I28 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G26">
-        <f>if(Sheet1!H28 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
+        <f>IF(Sheet1!H28 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>Sheet1!A29</f>
         <v>27</v>
@@ -3397,15 +3718,15 @@
         <v>1999</v>
       </c>
       <c r="F27">
-        <f>if(Sheet1!I29 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I29 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G27">
-        <f>if(Sheet1!H29 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28">
+        <f>IF(Sheet1!H29 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>Sheet1!A30</f>
         <v>28</v>
@@ -3427,15 +3748,15 @@
         <v>1999</v>
       </c>
       <c r="F28">
-        <f>if(Sheet1!I30 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I30 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G28">
-        <f>if(Sheet1!H30 = "passiv",0,1)</f>
+        <f>IF(Sheet1!H30 = "passiv",0,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>Sheet1!A31</f>
         <v>29</v>
@@ -3457,15 +3778,15 @@
         <v>1980</v>
       </c>
       <c r="F29">
-        <f>if(Sheet1!I31 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I31 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G29">
-        <f>if(Sheet1!H31 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30">
+        <f>IF(Sheet1!H31 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>Sheet1!A32</f>
         <v>30</v>
@@ -3487,15 +3808,15 @@
         <v>1985</v>
       </c>
       <c r="F30">
-        <f>if(Sheet1!I32 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I32 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G30">
-        <f>if(Sheet1!H32 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
+        <f>IF(Sheet1!H32 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>Sheet1!A33</f>
         <v>31</v>
@@ -3517,15 +3838,15 @@
         <v>1990</v>
       </c>
       <c r="F31">
-        <f>if(Sheet1!I33 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I33 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G31">
-        <f>if(Sheet1!H33 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
+        <f>IF(Sheet1!H33 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>Sheet1!A34</f>
         <v>32</v>
@@ -3547,15 +3868,15 @@
         <v>1950</v>
       </c>
       <c r="F32">
-        <f>if(Sheet1!I34 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I34 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G32">
-        <f>if(Sheet1!H34 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
+        <f>IF(Sheet1!H34 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>Sheet1!A35</f>
         <v>33</v>
@@ -3577,15 +3898,15 @@
         <v>1955</v>
       </c>
       <c r="F33">
-        <f>if(Sheet1!I35 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I35 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G33">
-        <f>if(Sheet1!H35 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
+        <f>IF(Sheet1!H35 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>Sheet1!A36</f>
         <v>34</v>
@@ -3607,15 +3928,15 @@
         <v>1958</v>
       </c>
       <c r="F34">
-        <f>if(Sheet1!I36 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I36 = "motionist",2,1)</f>
         <v>2</v>
       </c>
       <c r="G34">
-        <f>if(Sheet1!H36 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35">
+        <f>IF(Sheet1!H36 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>Sheet1!A37</f>
         <v>35</v>
@@ -3637,15 +3958,15 @@
         <v>1959</v>
       </c>
       <c r="F35">
-        <f>if(Sheet1!I37 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I37 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G35">
-        <f>if(Sheet1!H37 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36">
+        <f>IF(Sheet1!H37 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>Sheet1!A38</f>
         <v>36</v>
@@ -3667,15 +3988,15 @@
         <v>1980</v>
       </c>
       <c r="F36">
-        <f>if(Sheet1!I38 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I38 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G36">
-        <f>if(Sheet1!H38 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37">
+        <f>IF(Sheet1!H38 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>Sheet1!A39</f>
         <v>37</v>
@@ -3697,15 +4018,15 @@
         <v>1985</v>
       </c>
       <c r="F37">
-        <f>if(Sheet1!I39 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I39 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G37">
-        <f>if(Sheet1!H39 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38">
+        <f>IF(Sheet1!H39 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38">
         <f>Sheet1!A40</f>
         <v>38</v>
@@ -3727,15 +4048,15 @@
         <v>1990</v>
       </c>
       <c r="F38">
-        <f>if(Sheet1!I40 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I40 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G38">
-        <f>if(Sheet1!H40 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39">
+        <f>IF(Sheet1!H40 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39">
         <f>Sheet1!A41</f>
         <v>39</v>
@@ -3757,15 +4078,15 @@
         <v>1950</v>
       </c>
       <c r="F39">
-        <f>if(Sheet1!I41 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I41 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G39">
-        <f>if(Sheet1!H41 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40">
+        <f>IF(Sheet1!H41 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40">
         <f>Sheet1!A42</f>
         <v>40</v>
@@ -3787,15 +4108,15 @@
         <v>1955</v>
       </c>
       <c r="F40">
-        <f>if(Sheet1!I42 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I42 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G40">
-        <f>if(Sheet1!H42 = "passiv",0,1)</f>
+        <f>IF(Sheet1!H42 = "passiv",0,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41">
         <f>Sheet1!A43</f>
         <v>41</v>
@@ -3817,15 +4138,15 @@
         <v>1958</v>
       </c>
       <c r="F41">
-        <f>if(Sheet1!I43 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I43 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G41">
-        <f>if(Sheet1!H43 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42">
+        <f>IF(Sheet1!H43 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42">
         <f>Sheet1!A44</f>
         <v>42</v>
@@ -3847,15 +4168,15 @@
         <v>1959</v>
       </c>
       <c r="F42">
-        <f>if(Sheet1!I44 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I44 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G42">
-        <f>if(Sheet1!H44 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43">
+        <f>IF(Sheet1!H44 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43">
         <f>Sheet1!A45</f>
         <v>43</v>
@@ -3877,15 +4198,15 @@
         <v>2002</v>
       </c>
       <c r="F43">
-        <f>if(Sheet1!I45 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I45 = "motionist",2,1)</f>
         <v>2</v>
       </c>
       <c r="G43">
-        <f>if(Sheet1!H45 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
+        <f>IF(Sheet1!H45 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44">
         <f>Sheet1!A46</f>
         <v>44</v>
@@ -3907,15 +4228,15 @@
         <v>2005</v>
       </c>
       <c r="F44">
-        <f>if(Sheet1!I46 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I46 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G44">
-        <f>if(Sheet1!H46 = "passiv",0,1)</f>
+        <f>IF(Sheet1!H46 = "passiv",0,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45">
         <f>Sheet1!A47</f>
         <v>45</v>
@@ -3937,15 +4258,15 @@
         <v>1999</v>
       </c>
       <c r="F45">
-        <f>if(Sheet1!I47 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I47 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G45">
-        <f>if(Sheet1!H47 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46">
+        <f>IF(Sheet1!H47 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46">
         <f>Sheet1!A48</f>
         <v>46</v>
@@ -3967,15 +4288,15 @@
         <v>1999</v>
       </c>
       <c r="F46">
-        <f>if(Sheet1!I48 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I48 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G46">
-        <f>if(Sheet1!H48 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47">
+        <f>IF(Sheet1!H48 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47">
         <f>Sheet1!A49</f>
         <v>47</v>
@@ -3997,15 +4318,15 @@
         <v>1998</v>
       </c>
       <c r="F47">
-        <f>if(Sheet1!I49 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I49 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G47">
-        <f>if(Sheet1!H49 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48">
+        <f>IF(Sheet1!H49 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48">
         <f>Sheet1!A50</f>
         <v>48</v>
@@ -4027,15 +4348,15 @@
         <v>1995</v>
       </c>
       <c r="F48">
-        <f>if(Sheet1!I50 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I50 = "motionist",2,1)</f>
         <v>1</v>
       </c>
       <c r="G48">
-        <f>if(Sheet1!H50 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49">
+        <f>IF(Sheet1!H50 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49">
         <f>Sheet1!A51</f>
         <v>49</v>
@@ -4057,103 +4378,103 @@
         <v>2004</v>
       </c>
       <c r="F49">
-        <f>if(Sheet1!I51 = "motionist",2,1)</f>
+        <f>IF(Sheet1!I51 = "motionist",2,1)</f>
         <v>2</v>
       </c>
       <c r="G49">
-        <f>if(Sheet1!H51 = "passiv",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
+        <f>IF(Sheet1!H51 = "passiv",0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50">
         <f>Sheet1!A52</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B50" t="str">
         <f>Sheet1!B52 &amp; " " &amp; Sheet1!C52</f>
-        <v> </v>
-      </c>
-      <c r="C50" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C50">
         <f>Sheet1!D52</f>
-        <v/>
-      </c>
-      <c r="D50" t="str">
+        <v>0</v>
+      </c>
+      <c r="D50">
         <f>Sheet1!E52</f>
-        <v/>
-      </c>
-      <c r="E50" t="str">
+        <v>0</v>
+      </c>
+      <c r="E50">
         <f>Sheet1!J52</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51">
         <f>Sheet1!A53</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B51" t="str">
         <f>Sheet1!B53 &amp; " " &amp; Sheet1!C53</f>
-        <v> </v>
-      </c>
-      <c r="C51" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C51">
         <f>Sheet1!D53</f>
-        <v/>
-      </c>
-      <c r="D51" t="str">
+        <v>0</v>
+      </c>
+      <c r="D51">
         <f>Sheet1!E53</f>
-        <v/>
-      </c>
-      <c r="E51" t="str">
+        <v>0</v>
+      </c>
+      <c r="E51">
         <f>Sheet1!J53</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52">
         <f>Sheet1!A54</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B52" t="str">
         <f>Sheet1!B54 &amp; " " &amp; Sheet1!C54</f>
-        <v> </v>
-      </c>
-      <c r="C52" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C52">
         <f>Sheet1!D54</f>
-        <v/>
-      </c>
-      <c r="D52" t="str">
+        <v>0</v>
+      </c>
+      <c r="D52">
         <f>Sheet1!E54</f>
-        <v/>
-      </c>
-      <c r="E52" t="str">
+        <v>0</v>
+      </c>
+      <c r="E52">
         <f>Sheet1!J54</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53">
         <f>Sheet1!A55</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B53" t="str">
         <f>Sheet1!B55 &amp; " " &amp; Sheet1!C55</f>
-        <v> </v>
-      </c>
-      <c r="C53" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C53">
         <f>Sheet1!D55</f>
-        <v/>
-      </c>
-      <c r="D53" t="str">
+        <v>0</v>
+      </c>
+      <c r="D53">
         <f>Sheet1!E55</f>
-        <v/>
-      </c>
-      <c r="E53" t="str">
+        <v>0</v>
+      </c>
+      <c r="E53">
         <f>Sheet1!J55</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>